<commit_message>
Add new commands to support carving
1.AGM.Modelling.CreateTextSheet
2.AGM.Modelling.SweepByDist
3.AGM.Modelling.IntersectHollowCylinder
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="255">
   <si>
     <t>日期</t>
   </si>
@@ -1885,6 +1885,78 @@
     <t>AGM.Modelling.GetBodyFaces(ModelObject)
 得到一个body上所有的面
 范例：set_entity_color.js</t>
+  </si>
+  <si>
+    <t>text (string): 输入的文本</t>
+  </si>
+  <si>
+    <t>fontsize (double): 输入的字体大小</t>
+  </si>
+  <si>
+    <t>xlength\ylength (double): 用于限制字体轮廓的方框的长度和宽度（见下图）</t>
+  </si>
+  <si>
+    <t>target_origin (Position)\ target_x_axis (Vector)\target_y_axis (Vector): 定义了一个局部坐标系用来放置字体轮廓，xlength是方框在x轴的长度，ylength是方框在y轴的长度</t>
+  </si>
+  <si>
+    <t>out ModelObject: 输出的字体轮廓</t>
+  </si>
+  <si>
+    <t>wrap (bool) : 可不填，wrap默认为false。wrap = true和false的区别如下面两张图所示，这两张图除了wrap的值以前其他的参数一样。wrap = true的时候为了让字体轮廓充满方框，字体可能变形。</t>
+  </si>
+  <si>
+    <t>新增：
+1. AGM.Modelling.CreateTextSheet
+//AGM.Modelling.CreateTextSheet( text, fontname, fontsize, xlength, ylength, target_origin, target_x_axis, target_y_axis, wrap, out textObject)
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\planar_text.js, js_files\cylindrical_text.js）
+创建刻字轮廓
+2. AGM.Modelling.SweepByDist
+//AGM.Modelling.SweepByDist( in\out profile, distance, bothside )
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\planar_text.js, js_files\cylindrical_text.js）
+字体轮廓拉伸
+3. AGM.Modelling.IntersectHollowCylinder
+//AGM.Modelling.IntersectHollowCylinder( in\out Modelbody, bottom_position, top_position, max_radius, min_radius )
+（命令参数参考js_files\radf_init.js，命令使用参考js_files\cylindrical_text.js）
+用空心圆柱对字体轮廓进行裁剪，用于圆柱面刻字</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.CreateTextSheet( text, fontname, fontsize, xlength, ylength, target_origin, target_x_axis, target_y_axis, wrap, out ModelObject);
+创建刻字轮廓
+范例: planar_text.js, cylindrical_text.js</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.SweepByDist( in\out profile, distance, bothside );
+字体轮廓沿局部坐标系的z轴方向拉伸
+范例: planar_text.js, cylindrical_text.js</t>
+  </si>
+  <si>
+    <t>in\out profile (ModelObject) : 输入的字体轮廓</t>
+  </si>
+  <si>
+    <t>distance (double): 沿局部坐标系的z轴方向拉伸的长度</t>
+  </si>
+  <si>
+    <t>bothside (bool): 可以不填，默认是fasle，用来表示是否正负方向同时拉伸</t>
+  </si>
+  <si>
+    <t>fontname (string): 输入的字体名称</t>
+  </si>
+  <si>
+    <t>bottom_position (Position): 空心圆柱轴线的起点</t>
+  </si>
+  <si>
+    <t>top_position (Position): 空心圆柱轴线的终点</t>
+  </si>
+  <si>
+    <t>max_radius (double): 空心圆柱的外径</t>
+  </si>
+  <si>
+    <t>min_radius (double): 空心圆柱的内径，可不填，不填表示实心圆柱</t>
+  </si>
+  <si>
+    <t>AGM.Modelling.IntersectHollowCylinder( in\out Modelbody, bottom_position, top_position, max_radius, min_radius );
+用空心圆柱对字体轮廓进行裁剪
+范例: cylindrical_text.js</t>
   </si>
 </sst>
 </file>
@@ -2142,7 +2214,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>957119</xdr:colOff>
+      <xdr:colOff>294511</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>2982</xdr:rowOff>
     </xdr:to>
@@ -2260,6 +2332,82 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1540771</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>32143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2015192</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>166889</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4124945" y="49270595"/>
+          <a:ext cx="5503621" cy="2361111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2525157</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>904048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2260474</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>48781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10138531" y="49228100"/>
+          <a:ext cx="6268639" cy="2285498"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2554,10 +2702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2864,7 +3012,7 @@
     </row>
     <row r="38" spans="1:2" ht="129.6">
       <c r="A38" s="1">
-        <v>20190313</v>
+        <v>20200313</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>220</v>
@@ -2872,7 +3020,7 @@
     </row>
     <row r="39" spans="1:2" ht="100.8">
       <c r="A39" s="1">
-        <v>20190314</v>
+        <v>20200314</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>226</v>
@@ -2880,7 +3028,7 @@
     </row>
     <row r="40" spans="1:2" ht="72">
       <c r="A40" s="1">
-        <v>20190318</v>
+        <v>20200318</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>227</v>
@@ -2888,10 +3036,18 @@
     </row>
     <row r="41" spans="1:2" ht="144">
       <c r="A41" s="1">
-        <v>20190327</v>
+        <v>20200327</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="201.6">
+      <c r="A42" s="1">
+        <v>20200416</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2902,10 +3058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2916,8 +3072,9 @@
     <col min="4" max="4" width="38.5546875" customWidth="1"/>
     <col min="5" max="5" width="56.6640625" customWidth="1"/>
     <col min="6" max="6" width="41.77734375" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" customWidth="1"/>
+    <col min="8" max="8" width="65.6640625" customWidth="1"/>
+    <col min="9" max="9" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -4487,6 +4644,269 @@
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
+    </row>
+    <row r="85" spans="1:13" ht="86.4">
+      <c r="A85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="J85" s="11"/>
+      <c r="K85" s="11"/>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+    </row>
+    <row r="100" spans="1:11" ht="57.6">
+      <c r="A100" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="10"/>
+      <c r="K100" s="10"/>
+    </row>
+    <row r="101" spans="1:11" ht="72">
+      <c r="A101" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="H101" s="11"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="10"/>
+      <c r="K101" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add draft angle in AGM.Modelling.SweepByDist
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="257">
   <si>
     <t>日期</t>
   </si>
@@ -1925,11 +1925,6 @@
 范例: planar_text.js, cylindrical_text.js</t>
   </si>
   <si>
-    <t>AGM.Modelling.SweepByDist( in\out profile, distance, bothside );
-字体轮廓沿局部坐标系的z轴方向拉伸
-范例: planar_text.js, cylindrical_text.js</t>
-  </si>
-  <si>
     <t>in\out profile (ModelObject) : 输入的字体轮廓</t>
   </si>
   <si>
@@ -1957,6 +1952,48 @@
     <t>AGM.Modelling.IntersectHollowCylinder( in\out Modelbody, bottom_position, top_position, max_radius, min_radius );
 用空心圆柱对字体轮廓进行裁剪
 范例: cylindrical_text.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">修改：
+AGM.Modelling.SweepByDist
+//AGM.Modelling.SweepByDist( in\out profile, distance, bothside = false, draftangle = 0 )
+新增加了一个参数拔模角度draftangle.
+第三个参数bothside默认是false，第四个参数draftangle默认是0.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">用户如果要设置第四个参数draftangle，必须先设置第三个参数bothside.
+draftangle的输入参数是拔模角度，如果是正数，横截面沿着拉伸方向越来越小；如果是负数，横截面沿着拉伸方向越来越大
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（命令参数参考js_files\radf_init.js，命令使用参考js_files\planar_text.js）</t>
+    </r>
+  </si>
+  <si>
+    <t>AGM.Modelling.SweepByDist( in\out profile, distance, bothside = false, draftangle = 0 );
+字体轮廓沿局部坐标系的z轴方向拉伸
+范例: planar_text.js, cylindrical_text.js</t>
+  </si>
+  <si>
+    <t>draftangle (double): 
+拔模角度，默认为0
+用户如果要设置第四个参数draftangle，必须先设置第三个参数bothside.
+draftangle如果是正数，横截面沿着拉伸方向越来越小；如果是负数，横截面沿着拉伸方向越来越大</t>
   </si>
 </sst>
 </file>
@@ -2702,10 +2739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3050,6 +3087,23 @@
         <v>243</v>
       </c>
     </row>
+    <row r="43" spans="1:2" ht="115.2">
+      <c r="A43" s="1">
+        <v>20200506</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3060,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="E93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3071,7 +3125,7 @@
     <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="38.5546875" customWidth="1"/>
     <col min="5" max="5" width="56.6640625" customWidth="1"/>
-    <col min="6" max="6" width="41.77734375" customWidth="1"/>
+    <col min="6" max="6" width="69" customWidth="1"/>
     <col min="7" max="7" width="33.5546875" customWidth="1"/>
     <col min="8" max="8" width="65.6640625" customWidth="1"/>
     <col min="9" max="9" width="44.33203125" customWidth="1"/>
@@ -4656,7 +4710,7 @@
         <v>237</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>238</v>
@@ -4858,23 +4912,25 @@
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
     </row>
-    <row r="100" spans="1:11" ht="57.6">
+    <row r="100" spans="1:11" ht="72">
       <c r="A100" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="D100" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="E100" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E100" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="F100" s="11"/>
+      <c r="F100" s="11" t="s">
+        <v>256</v>
+      </c>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
       <c r="I100" s="11"/>
@@ -4886,22 +4942,22 @@
         <v>6</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D101" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E101" s="11" t="s">
+      <c r="F101" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="G101" s="11" t="s">
         <v>252</v>
-      </c>
-      <c r="G101" s="11" t="s">
-        <v>253</v>
       </c>
       <c r="H101" s="11"/>
       <c r="I101" s="11"/>

</xml_diff>